<commit_message>
Release, Rezonit DRC done
</commit_message>
<xml_diff>
--- a/Project Outputs for DCDC_SAUVC26_PCB/ГИДР.123456.014-01.02/Документация/ГИДР.123456.014-01.02 ПЭ3.xlsx
+++ b/Project Outputs for DCDC_SAUVC26_PCB/ГИДР.123456.014-01.02/Документация/ГИДР.123456.014-01.02 ПЭ3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1\AppData\Local\TempReleases\Snapshot\1\Assembly 02\Документация\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E864D7AD-5CBF-4FD9-AF76-46523228E6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CFF7F60-148A-49AA-99F5-BB0D8E600CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BAC53062-0416-42C5-A444-3902CA2F08D2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C1A0C2CC-FC7C-45FA-900C-DCC3CB37997D}"/>
   </bookViews>
   <sheets>
     <sheet name="ГИДР.123456.014-01.02 ПЭ3" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="168">
   <si>
     <t>Line #</t>
   </si>
@@ -908,7 +908,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8C0E03D-F028-4A1F-A9A7-AB765B23065D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4FC4F6E-79F2-4E82-B296-EE1BAD90B8F4}">
   <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1688,7 +1688,9 @@
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
+      <c r="A32" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="B32" s="2" t="s">
         <v>85</v>
       </c>
@@ -1710,7 +1712,9 @@
       <c r="L32" s="1"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
+      <c r="A33" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="B33" s="2" t="s">
         <v>85</v>
       </c>
@@ -2020,7 +2024,9 @@
       <c r="L45" s="1"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A46" s="1"/>
+      <c r="A46" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="B46" s="2" t="s">
         <v>85</v>
       </c>

</xml_diff>